<commit_message>
first resutlts + upgrade langchain versionning + create package
</commit_message>
<xml_diff>
--- a/pythonv2/results/response_excel/responses.xlsx
+++ b/pythonv2/results/response_excel/responses.xlsx
@@ -1,25 +1,99 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blevraultgroup-my.sharepoint.com/personal/marius_pingaud_berger-levrault_com/Documents/Bureau/Sorbonne/M2/Master thesis/Requirement Engineering/master_thesis_xp/pythonv2/results/response_excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_AD4D9D64A577C15A4A54188D781E63C45BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8CF8ECA-9F0C-4F58-9A54-A04598FEC106}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="RQ1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+  <si>
+    <t>eTour</t>
+  </si>
+  <si>
+    <t>iTrust</t>
+  </si>
+  <si>
+    <t>Albergate</t>
+  </si>
+  <si>
+    <t>F1 score</t>
+  </si>
+  <si>
+    <t>Correct Matches</t>
+  </si>
+  <si>
+    <t>with_only_code</t>
+  </si>
+  <si>
+    <t>Wanted Links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Total Given</t>
+  </si>
+  <si>
+    <t>% correct matches</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -45,17 +119,248 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +371,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8EDBC4B4-639B-4772-9246-3F92633C6CE2}" name="Tableau1" displayName="Tableau1" ref="G5:J9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="G5:J9" xr:uid="{8EDBC4B4-639B-4772-9246-3F92633C6CE2}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{2AE86955-5798-4F53-944E-C4AEAE0C26C5}" name="with_only_code" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{CB44D13F-E14C-42CC-85F2-95DFA9C0A213}" name="eTour" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{5739C6E6-A1DC-4075-85F7-8F23A7ECB5DC}" name="iTrust" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C26F2C11-B71F-4B3C-A052-7F87436BD110}" name="Albergate" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9096F76B-227C-4769-A426-FD98EEC0017F}" name="Tableau2" displayName="Tableau2" ref="B5:E6" totalsRowShown="0">
+  <autoFilter ref="B5:E6" xr:uid="{9096F76B-227C-4769-A426-FD98EEC0017F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A30D5633-D271-4AF1-B193-F0BA60A542FE}" name="  "/>
+    <tableColumn id="2" xr3:uid="{88800BA8-DB54-44BA-8CC5-B23337137D10}" name="eTour"/>
+    <tableColumn id="3" xr3:uid="{39990FC0-181A-4E65-B2AB-EA1C67BB4259}" name="iTrust"/>
+    <tableColumn id="4" xr3:uid="{16D7F4D2-F33E-45D7-A62C-E6FFF02ABC61}" name="Albergate"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +661,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B5:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>308</v>
+      </c>
+      <c r="D6">
+        <v>418</v>
+      </c>
+      <c r="E6">
+        <v>54</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="8">
+        <v>143</v>
+      </c>
+      <c r="I7" s="8">
+        <v>163</v>
+      </c>
+      <c r="J7" s="9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1" cm="1">
+        <f t="array" ref="H8">H7/Tableau2[eTour]*100</f>
+        <v>46.428571428571431</v>
+      </c>
+      <c r="I8" s="1" cm="1">
+        <f t="array" ref="I8">I7/Tableau2[iTrust]*100</f>
+        <v>38.995215311004785</v>
+      </c>
+      <c r="J8" s="3" cm="1">
+        <f t="array" ref="J8">J7/Tableau2[Albergate]*100</f>
+        <v>87.037037037037038</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1">
+        <v>284</v>
+      </c>
+      <c r="I9" s="1">
+        <v>474</v>
+      </c>
+      <c r="J9" s="3">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new results + f1 score update
</commit_message>
<xml_diff>
--- a/pythonv2/results/response_excel/responses.xlsx
+++ b/pythonv2/results/response_excel/responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blevraultgroup-my.sharepoint.com/personal/marius_pingaud_berger-levrault_com/Documents/Bureau/Sorbonne/M2/Master thesis/Requirement Engineering/master_thesis_xp/pythonv2/results/response_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="6_{D18F53DD-BD7E-4EFC-B763-D1CA351000E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AB7C680-0961-4067-B74B-E36367F77DEE}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="6_{D18F53DD-BD7E-4EFC-B763-D1CA351000E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8174C1A-62BD-4350-9321-53CD49DBEDC0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t>eTour</t>
   </si>
@@ -157,6 +156,39 @@
   </si>
   <si>
     <t>with_code</t>
+  </si>
+  <si>
+    <t>with_all_generated_comment</t>
+  </si>
+  <si>
+    <t>0.4412</t>
+  </si>
+  <si>
+    <t>0.2715</t>
+  </si>
+  <si>
+    <t>0.2623</t>
+  </si>
+  <si>
+    <t>0.0974</t>
+  </si>
+  <si>
+    <t>0.3254</t>
+  </si>
+  <si>
+    <t>0.5926</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>0.1594</t>
+  </si>
+  <si>
+    <t>0.2960</t>
+  </si>
+  <si>
+    <t>0.3633</t>
   </si>
 </sst>
 </file>
@@ -217,6 +249,21 @@
   </cellStyles>
   <dxfs count="20">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -271,18 +318,97 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -303,100 +429,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -411,13 +443,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8EDBC4B4-639B-4772-9246-3F92633C6CE2}" name="Tableau1" displayName="Tableau1" ref="G5:J11" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8EDBC4B4-639B-4772-9246-3F92633C6CE2}" name="Tableau1" displayName="Tableau1" ref="G5:J11" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="G5:J11" xr:uid="{8EDBC4B4-639B-4772-9246-3F92633C6CE2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2AE86955-5798-4F53-944E-C4AEAE0C26C5}" name="with_code" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{CB44D13F-E14C-42CC-85F2-95DFA9C0A213}" name="eTour" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{5739C6E6-A1DC-4075-85F7-8F23A7ECB5DC}" name="iTrust" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{C26F2C11-B71F-4B3C-A052-7F87436BD110}" name="Albergate" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{2AE86955-5798-4F53-944E-C4AEAE0C26C5}" name="with_code" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{CB44D13F-E14C-42CC-85F2-95DFA9C0A213}" name="eTour" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{5739C6E6-A1DC-4075-85F7-8F23A7ECB5DC}" name="iTrust" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{C26F2C11-B71F-4B3C-A052-7F87436BD110}" name="Albergate" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -437,28 +469,41 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D98C44C1-0B5B-4289-8A49-4667B3FBDF17}" name="Tableau3" displayName="Tableau3" ref="G13:J19" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D98C44C1-0B5B-4289-8A49-4667B3FBDF17}" name="Tableau3" displayName="Tableau3" ref="G13:J19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="G13:J19" xr:uid="{D98C44C1-0B5B-4289-8A49-4667B3FBDF17}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E7FCE47E-2275-45CB-B319-147352933C39}" name="with_code_comment" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{51DDBC57-69F3-48F7-8830-FCEF1AAE1500}" name="eTour" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{85572FF5-FF13-4FEE-A08D-2F467C221025}" name="iTrust" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{7EB03A88-C7CE-4355-99DE-2EFC52B37BC1}" name="Albergate" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{E7FCE47E-2275-45CB-B319-147352933C39}" name="with_code_comment" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{51DDBC57-69F3-48F7-8830-FCEF1AAE1500}" name="eTour" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{85572FF5-FF13-4FEE-A08D-2F467C221025}" name="iTrust" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{7EB03A88-C7CE-4355-99DE-2EFC52B37BC1}" name="Albergate" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{118F3364-9537-4BDF-8BE3-CD5C6EE96565}" name="Tableau6" displayName="Tableau6" ref="G22:J28" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{118F3364-9537-4BDF-8BE3-CD5C6EE96565}" name="Tableau6" displayName="Tableau6" ref="G22:J28" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="G22:J28" xr:uid="{118F3364-9537-4BDF-8BE3-CD5C6EE96565}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{035DB747-2B1B-4729-AE9E-C4AD735DB79D}" name="with_one_comment" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{A1210D52-A3E2-482D-9209-00AAD95FA4F9}" name="eTour" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{51FE4424-30A5-4026-9E4A-47319F9C40E4}" name="iTrust" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{FD2F01BF-3C4C-46E4-B10F-63ABA631F3C2}" name="Albergate" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{035DB747-2B1B-4729-AE9E-C4AD735DB79D}" name="with_one_comment" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A1210D52-A3E2-482D-9209-00AAD95FA4F9}" name="eTour" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{51FE4424-30A5-4026-9E4A-47319F9C40E4}" name="iTrust" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{FD2F01BF-3C4C-46E4-B10F-63ABA631F3C2}" name="Albergate" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{67A10623-EB36-4284-843F-216B3A3DFE9E}" name="Tableau4" displayName="Tableau4" ref="G30:J36" totalsRowShown="0">
+  <autoFilter ref="G30:J36" xr:uid="{67A10623-EB36-4284-843F-216B3A3DFE9E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7B639B08-BBD7-418A-971C-7718A3003F1A}" name="with_all_generated_comment"/>
+    <tableColumn id="2" xr3:uid="{3F5A7B4F-9A53-4AAF-9D47-265C27497AE4}" name="eTour"/>
+    <tableColumn id="3" xr3:uid="{078F3145-3F9A-4E02-B5ED-6077887BB2E1}" name="iTrust"/>
+    <tableColumn id="4" xr3:uid="{5C6FCB9A-FC93-48F1-9108-E619AEEFA59D}" name="Albergate"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -725,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:Q30"/>
+  <dimension ref="B5:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,18 +1189,115 @@
       <c r="Q29" s="2"/>
     </row>
     <row r="30" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>2</v>
+      </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
     </row>
+    <row r="31" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31">
+        <v>30</v>
+      </c>
+      <c r="I31">
+        <v>136</v>
+      </c>
+      <c r="J31">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <v>68</v>
+      </c>
+      <c r="I32">
+        <v>501</v>
+      </c>
+      <c r="J32">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>308</v>
+      </c>
+      <c r="I33">
+        <v>418</v>
+      </c>
+      <c r="J33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G36" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>